<commit_message>
adding process edit address page
</commit_message>
<xml_diff>
--- a/Doc/set up enviroment.xlsx
+++ b/Doc/set up enviroment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecommerce web\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Meos-Shop\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DE6F09-E943-4AE1-8E97-FD5C281297D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2495E19-A3B4-4A07-B348-9C85D937580E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AC654E24-17D1-43BB-B540-0F1C915667C6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>npm i</t>
   </si>
@@ -126,8 +126,14 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>LOCAL_URL=</t>
+    <t>password: 12345</t>
+  </si>
+  <si>
+    <t>accopunt: admin</t>
+  </si>
+  <si>
+    <r>
+      <t>LOCAL_URL_AD=</t>
     </r>
     <r>
       <rPr>
@@ -141,10 +147,19 @@
     </r>
   </si>
   <si>
-    <t>password: 12345</t>
-  </si>
-  <si>
-    <t>accopunt: admin</t>
+    <r>
+      <t>LOCAL_URL_CL=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>http://localhost:3005</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -518,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0CBF731-8210-4AF1-AF44-323A61B4743A}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,51 +572,50 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -609,33 +623,39 @@
       </c>
       <c r="B18" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>